<commit_message>
Fixed Connectors and uploaded new Gerber Files
</commit_message>
<xml_diff>
--- a/Rev 1.1/PowerDistro BOM_2019-2020.xlsx
+++ b/Rev 1.1/PowerDistro BOM_2019-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurta\Desktop\UW Seattle\19-20 Husky Robotics\REV 1\Chassis-Power-Distro-PCB-A-2019-2020\Rev 1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95492455-D7BA-4EDA-9BB9-67FA2A8A39D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A3180D-B0F8-4317-BDF9-1847C935B91B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1292,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91CBD03B-EE9F-4C55-837D-AF17F6E98A83}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.7"/>

</xml_diff>